<commit_message>
[/] textual changes to PVA
</commit_message>
<xml_diff>
--- a/Documentatie/Planning.xlsx
+++ b/Documentatie/Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Project-CCSB\Documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Desktop\CCSB\Project-CCSB\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69A68AFD-DAC8-49BF-B02F-9AF4D5C045C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D59DB-FE57-4AE2-B9E8-DF9CFA414313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Projectplanner</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Oplevering</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -943,6 +946,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -954,27 +978,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1425,10 +1428,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO31"/>
+  <dimension ref="B1:BV31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BV1" sqref="BV1:BV1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1440,7 +1443,7 @@
     <col min="8" max="27" width="2.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:74" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1449,15 +1452,18 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="BV1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="2:74" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1465,25 +1471,25 @@
         <v>1</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="15"/>
-      <c r="R2" s="29" t="s">
+      <c r="R2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
       <c r="Z2" s="16"/>
       <c r="AA2" s="20" t="s">
         <v>12</v>
@@ -1492,47 +1498,47 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="22"/>
       <c r="AE2" s="17"/>
-      <c r="AF2" s="31" t="s">
+      <c r="AF2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="18"/>
-      <c r="AP2" s="31" t="s">
+      <c r="AP2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-    </row>
-    <row r="3" spans="2:67" s="10" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+      <c r="AU2" s="29"/>
+      <c r="AV2" s="29"/>
+      <c r="AW2" s="29"/>
+      <c r="AX2" s="29"/>
+    </row>
+    <row r="3" spans="2:74" s="10" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="19" t="s">
@@ -1558,13 +1564,13 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+    <row r="4" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="32"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1746,8 +1752,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="6">
@@ -1766,8 +1772,8 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+    <row r="6" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="6">
@@ -1786,8 +1792,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="6">
@@ -1806,8 +1812,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="6">
@@ -1826,8 +1832,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
+    <row r="9" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="6">
@@ -1846,8 +1852,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+    <row r="10" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="6">
@@ -1866,8 +1872,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="6">
@@ -1886,8 +1892,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
+    <row r="12" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="6">
@@ -1906,8 +1912,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33" t="s">
+    <row r="13" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="6">
@@ -1926,8 +1932,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+    <row r="14" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="6">
@@ -1946,8 +1952,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+    <row r="15" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="6">
@@ -1966,8 +1972,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+    <row r="16" spans="2:74" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="7">
@@ -1987,7 +1993,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="6">
@@ -2007,7 +2013,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6">
@@ -2027,11 +2033,11 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="6">
-        <v>7</v>
+      <c r="C19" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="6">
         <v>8</v>
@@ -2047,84 +2053,84 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="33"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="33"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="33"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="33"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="33"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="33"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="33"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="33"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="33"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="33"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="33"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="33"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -2132,17 +2138,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="AF2:AN2"/>
-    <mergeCell ref="AP2:AX2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="AF2:AN2"/>
+    <mergeCell ref="AP2:AX2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO31">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>